<commit_message>
revisi: tambah akurasi dan perbaikan decision tree
</commit_message>
<xml_diff>
--- a/assets/document/data-latih/Book3.xlsx
+++ b/assets/document/data-latih/Book3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arlan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C741025C-91EF-4019-AE9F-749D7E38D90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{304D077C-50DE-45CF-BE0A-4D9A7009BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27960" yWindow="-855" windowWidth="20700" windowHeight="11565" xr2:uid="{2BCAE969-05F2-4D1B-A7C5-35FA25D26809}"/>
+    <workbookView xWindow="-28920" yWindow="-3090" windowWidth="29040" windowHeight="16080" xr2:uid="{D7510696-5B87-4B97-9374-5CB0E78C7BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,154 +27,154 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
-    <t>SIMON SENA SOKA</t>
-  </si>
-  <si>
-    <t>Suryanda Mahesa Taka</t>
-  </si>
-  <si>
-    <t>Derrysto Rayfa1do Niab</t>
-  </si>
-  <si>
-    <t>EFRAT JOICE RATA</t>
-  </si>
-  <si>
-    <t>Gianti Maria Ange1a 2aridy Man</t>
-  </si>
-  <si>
-    <t>JEFREY CHRISTOFORUS 1AINAMA</t>
-  </si>
-  <si>
-    <t>Maria Magda1ena G1oria Jordan 1e1amu1a</t>
-  </si>
-  <si>
-    <t>YOHANES WI11IAM 1AOS</t>
-  </si>
-  <si>
-    <t>Vanya E1isabeth Muskanan</t>
-  </si>
-  <si>
-    <t>Grice1da Fabio1a Gusmao</t>
-  </si>
-  <si>
-    <t>Anti2as 2asca1is Gregorius Seran</t>
-  </si>
-  <si>
-    <t>BERTO1OMEUS DISMAS SOAR</t>
-  </si>
-  <si>
-    <t>ZA1VADOR 2. D. KOU</t>
-  </si>
-  <si>
-    <t>Frederikus Oni Seran</t>
-  </si>
-  <si>
-    <t>Rayna1do F. Renas Mbiru</t>
-  </si>
-  <si>
-    <t>Konradus Ko2ong Ba1a Wuwur</t>
-  </si>
-  <si>
-    <t>CHRISUA1DO JACOBUS 2U1O ERA2</t>
-  </si>
-  <si>
-    <t>KRISTOFFORUS AMASENE</t>
-  </si>
-  <si>
-    <t>Reina1do 1o2es De Sena</t>
-  </si>
-  <si>
-    <t>O1DY T.E. AMNIFU</t>
-  </si>
-  <si>
-    <t>Hamberd Banry Fa11o</t>
-  </si>
-  <si>
-    <t>JIMMY 2RABOWO SANDI 1I1Y</t>
-  </si>
-  <si>
-    <t>ERNESTO2 1ANGO TUKAN</t>
-  </si>
-  <si>
-    <t>Quido Suryadi Ngao</t>
-  </si>
-  <si>
-    <t>CHRISTINE AQUI1INA 1AKE</t>
-  </si>
-  <si>
-    <t>2ASCA1IS BEDA ADITYA ERA2</t>
-  </si>
-  <si>
-    <t>YOHANES YANSEN KO2ONG WITAK</t>
-  </si>
-  <si>
-    <t>Fransiskus Steven Du1i Manuk</t>
-  </si>
-  <si>
-    <t>ECBER RIVTO RICARDO VERISTO A1A</t>
-  </si>
-  <si>
-    <t>JUNINHO ROY RINA1DO FA1O</t>
-  </si>
-  <si>
-    <t>1UIS FRANSISCO JUNIOR 1EKI</t>
-  </si>
-  <si>
-    <t>RAFAE1 EVENTUS 1EKY</t>
-  </si>
-  <si>
-    <t>Markus Tehe Amannutur</t>
-  </si>
-  <si>
-    <t>RONIANTO 1O11O</t>
-  </si>
-  <si>
-    <t>Giancar1o Simon Satriani 1amane2a</t>
-  </si>
-  <si>
-    <t>Stivani N Wadhi</t>
-  </si>
-  <si>
-    <t>Yoandra Tubu1au</t>
-  </si>
-  <si>
-    <t>1UCKY ARFANDY YOHANES</t>
-  </si>
-  <si>
-    <t>Adrianus Nenoharan</t>
-  </si>
-  <si>
-    <t>JEFRI ARIYANTO KOFI</t>
-  </si>
-  <si>
-    <t>JANUARIO DA SI1VA FERNANDES</t>
-  </si>
-  <si>
-    <t>E2ifania Bachita 1o2es Soares</t>
-  </si>
-  <si>
-    <t>Sabino Jose Caet</t>
-  </si>
-  <si>
-    <t>E1utorio 1ourence Dos Reis</t>
-  </si>
-  <si>
-    <t>Veronika Maria Sone</t>
-  </si>
-  <si>
-    <t>NATACHYA E1MA 2UTRI A21UGI</t>
-  </si>
-  <si>
-    <t>Markus Young 1akamoa</t>
-  </si>
-  <si>
-    <t>Tobias De O1iveira</t>
-  </si>
-  <si>
-    <t>MARIA FEBRINTINA 1OWA DHUGE</t>
-  </si>
-  <si>
-    <t>Heribertus Kobo 2akae</t>
+    <t>Yulius Fernando Sado</t>
+  </si>
+  <si>
+    <t>Rex Chornelis Mbuilima</t>
+  </si>
+  <si>
+    <t>Klemens Marius BT</t>
+  </si>
+  <si>
+    <t>Lando Emeliano Sales Sonbay</t>
+  </si>
+  <si>
+    <t>Lando Emiliano Sales Sonbay</t>
+  </si>
+  <si>
+    <t>Thomas R. Pati Djaleng</t>
+  </si>
+  <si>
+    <t>Marisa Banunuh</t>
+  </si>
+  <si>
+    <t>Irvandisius Melkior Hasan</t>
+  </si>
+  <si>
+    <t>Edward Fendi Fahik</t>
+  </si>
+  <si>
+    <t>Sanry Melkias Ratu Edo</t>
+  </si>
+  <si>
+    <t>Ronaldo Santana Boro Tupen</t>
+  </si>
+  <si>
+    <t>Elton Petrus Maukolik</t>
+  </si>
+  <si>
+    <t>Blasedus Nahak</t>
+  </si>
+  <si>
+    <t>Guido Senu</t>
+  </si>
+  <si>
+    <t>Rivaldo Jong Nokas</t>
+  </si>
+  <si>
+    <t>Novriana Trivenia Mau</t>
+  </si>
+  <si>
+    <t>Ismael Simon Petrus Taneo</t>
+  </si>
+  <si>
+    <t>Syahidin Boleng Sanga</t>
+  </si>
+  <si>
+    <t>Fandy Thimotius Radja Udju</t>
+  </si>
+  <si>
+    <t>Maria Veliana Mone Djando</t>
+  </si>
+  <si>
+    <t>Maternus Dovanus Wake</t>
+  </si>
+  <si>
+    <t>Maria Veransia Rengi</t>
+  </si>
+  <si>
+    <t>Oktavianus Gili Dhou</t>
+  </si>
+  <si>
+    <t>Ochrin Stenly Erdipsen Hae Djingi</t>
+  </si>
+  <si>
+    <t>Anicetus Robertus Mangu Lewerang</t>
+  </si>
+  <si>
+    <t>CHRISLEEN STEFANYA VIRGINIO HERE</t>
+  </si>
+  <si>
+    <t>Hilarius Robinson Abes</t>
+  </si>
+  <si>
+    <t>Frederikus Halmon</t>
+  </si>
+  <si>
+    <t>Redeptus Fabiola Suri</t>
+  </si>
+  <si>
+    <t>Antonio Joao De Oliveira Tacae</t>
+  </si>
+  <si>
+    <t>Fransiskus Xaverius Igo Ruron</t>
+  </si>
+  <si>
+    <t>Bonar Fontura Setu Sale</t>
+  </si>
+  <si>
+    <t>Ana Freitas Guterres</t>
+  </si>
+  <si>
+    <t>Muhammad Zainudin S.S. Watun</t>
+  </si>
+  <si>
+    <t>Merita De Araujo Nascimento</t>
+  </si>
+  <si>
+    <t>Antonio Umbu Anjar Gusmao Nindir</t>
+  </si>
+  <si>
+    <t>ARIYANTO MOOY</t>
+  </si>
+  <si>
+    <t>Stefani Febrianti Sea Way</t>
+  </si>
+  <si>
+    <t>MARTINUS KURNIAWAN WILU</t>
+  </si>
+  <si>
+    <t>AURELIUS JULIANTO BARUNG</t>
+  </si>
+  <si>
+    <t>YOHANES PEHAN KELEN</t>
+  </si>
+  <si>
+    <t>Alfridus Jemianus Nahak</t>
+  </si>
+  <si>
+    <t>RUPERTUS DORECYANO BILLSHILA</t>
+  </si>
+  <si>
+    <t>MIKHAEL RANDY PAREIRA</t>
+  </si>
+  <si>
+    <t>FREDERIKUS JENTIUS LOGO DUE</t>
+  </si>
+  <si>
+    <t>SILVESTER LALISUC</t>
+  </si>
+  <si>
+    <t>AGUSTINUS ALLEUK ASURY</t>
+  </si>
+  <si>
+    <t>STEVANIA SANDARANA ELU</t>
+  </si>
+  <si>
+    <t>FRANSISKUS SALVI RUA</t>
+  </si>
+  <si>
+    <t>JULIANUS EDMUNDUS TAEK</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3644F239-51A4-440A-AD4C-294A6C9DC875}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED261B5-6379-44ED-BC40-93453F89C957}">
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -572,7 +572,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>22116001</v>
+        <v>22117076</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -581,27 +581,27 @@
         <v>1</v>
       </c>
       <c r="D1" s="2">
-        <v>2.44</v>
+        <v>2.61</v>
       </c>
       <c r="E1" s="2">
-        <v>1.94</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="F1" s="2">
-        <v>1.93</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="G1" s="2">
-        <v>1.49</v>
+        <v>1.92</v>
       </c>
       <c r="H1" s="3">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I1" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="J1" s="3">
         <v>0</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="3">
         <v>0</v>
       </c>
       <c r="L1" s="2">
@@ -613,7 +613,7 @@
     </row>
     <row r="2" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>22116002</v>
+        <v>22117078</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -622,39 +622,39 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>2.4700000000000002</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E2" s="2">
-        <v>1.31</v>
+        <v>2.31</v>
       </c>
       <c r="F2" s="2">
-        <v>1.65</v>
+        <v>2.37</v>
       </c>
       <c r="G2" s="2">
-        <v>1.28</v>
+        <v>2.17</v>
       </c>
       <c r="H2" s="3">
         <v>2</v>
       </c>
-      <c r="I2" s="2">
-        <v>0</v>
+      <c r="I2" s="3">
+        <v>2.5</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3</v>
+      </c>
+      <c r="M2" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>22116003</v>
+        <v>22117079</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -663,39 +663,39 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>1.84</v>
+        <v>3.23</v>
       </c>
       <c r="E3" s="2">
-        <v>1.47</v>
+        <v>3.1</v>
       </c>
       <c r="F3" s="2">
-        <v>1.71</v>
+        <v>3.16</v>
       </c>
       <c r="G3" s="2">
-        <v>1.91</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>3.07</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>22116004</v>
+        <v>22117080</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -704,80 +704,80 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>2.67</v>
+        <v>3.05</v>
       </c>
       <c r="E4" s="2">
-        <v>2.71</v>
+        <v>2.59</v>
       </c>
       <c r="F4" s="2">
-        <v>2.69</v>
+        <v>2.76</v>
       </c>
       <c r="G4" s="2">
-        <v>2.68</v>
+        <v>2.86</v>
       </c>
       <c r="H4" s="3">
-        <v>3.75</v>
+        <v>2</v>
       </c>
       <c r="I4" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L4" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>22116005</v>
+        <v>22117081</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>3.08</v>
+        <v>3.14</v>
       </c>
       <c r="E5" s="2">
-        <v>2.98</v>
+        <v>3.09</v>
       </c>
       <c r="F5" s="2">
-        <v>2.99</v>
+        <v>3.09</v>
       </c>
       <c r="G5" s="2">
-        <v>2.97</v>
+        <v>2.85</v>
       </c>
       <c r="H5" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="I5" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="J5" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K5" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="M5" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>22116006</v>
+        <v>22117084</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -786,80 +786,80 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>2.5</v>
+        <v>2.95</v>
       </c>
       <c r="E6" s="2">
-        <v>2.75</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F6" s="2">
-        <v>2.8</v>
+        <v>2.25</v>
       </c>
       <c r="G6" s="2">
-        <v>2.76</v>
+        <v>2.39</v>
       </c>
       <c r="H6" s="3">
         <v>2</v>
       </c>
       <c r="I6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K6" s="3">
         <v>2</v>
       </c>
       <c r="L6" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="M6" s="3">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="80.25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>22116007</v>
+        <v>22117085</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>3.31</v>
+        <v>3.07</v>
       </c>
       <c r="E7" s="2">
-        <v>3.3</v>
+        <v>2.98</v>
       </c>
       <c r="F7" s="2">
-        <v>3.29</v>
+        <v>3.06</v>
       </c>
       <c r="G7" s="2">
-        <v>3.21</v>
+        <v>3.01</v>
       </c>
       <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
         <v>3.5</v>
       </c>
-      <c r="I7" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="J7" s="3">
-        <v>2.5</v>
-      </c>
       <c r="K7" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="L7" s="3">
         <v>3</v>
       </c>
       <c r="M7" s="3">
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>22116008</v>
+        <v>22117087</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -868,121 +868,121 @@
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>3</v>
+        <v>2.52</v>
       </c>
       <c r="E8" s="2">
-        <v>3.06</v>
+        <v>2.39</v>
       </c>
       <c r="F8" s="2">
-        <v>2.96</v>
+        <v>2.27</v>
       </c>
       <c r="G8" s="2">
-        <v>2.87</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="H8" s="3">
         <v>2</v>
       </c>
       <c r="I8" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="J8" s="3">
-        <v>2</v>
+        <v>3.75</v>
       </c>
       <c r="K8" s="3">
-        <v>2</v>
-      </c>
-      <c r="L8" s="3">
-        <v>3.75</v>
+        <v>3</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>22116009</v>
+        <v>22117090</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>3.06</v>
+        <v>2.64</v>
       </c>
       <c r="E9" s="2">
-        <v>3.01</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F9" s="2">
-        <v>2.94</v>
+        <v>2.48</v>
       </c>
       <c r="G9" s="2">
-        <v>2.95</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="H9" s="3">
         <v>2</v>
       </c>
       <c r="I9" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="M9" s="3">
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>22116010</v>
+        <v>22117092</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>2.65</v>
+        <v>2.5</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>2.82</v>
+        <v>1.78</v>
       </c>
       <c r="G10" s="2">
-        <v>2.82</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
+        <v>2.13</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
       </c>
       <c r="I10" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
       </c>
       <c r="K10" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L10" s="3">
         <v>2</v>
       </c>
       <c r="M10" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>22116011</v>
+        <v>22117093</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -991,39 +991,39 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>2.83</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2">
-        <v>1.57</v>
+        <v>2.73</v>
       </c>
       <c r="F11" s="2">
-        <v>1.75</v>
+        <v>1.78</v>
       </c>
       <c r="G11" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>2.81</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>22116012</v>
+        <v>22117094</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -1032,39 +1032,39 @@
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>3.19</v>
+        <v>2.41</v>
       </c>
       <c r="E12" s="2">
-        <v>3.24</v>
+        <v>2.15</v>
       </c>
       <c r="F12" s="2">
-        <v>3.18</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2">
-        <v>3.11</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H12" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J12" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K12" s="3">
         <v>2</v>
       </c>
       <c r="L12" s="3">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="M12" s="3">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>22116013</v>
+        <v>22117095</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1073,39 +1073,39 @@
         <v>1</v>
       </c>
       <c r="D13" s="2">
-        <v>1.55</v>
+        <v>2.98</v>
       </c>
       <c r="E13" s="2">
-        <v>1.55</v>
+        <v>2.48</v>
       </c>
       <c r="F13" s="2">
-        <v>1.75</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="G13" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2.72</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>22116014</v>
+        <v>22117096</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1114,39 +1114,39 @@
         <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>1.17</v>
+        <v>3.05</v>
       </c>
       <c r="E14" s="2">
-        <v>1.75</v>
+        <v>3.1</v>
       </c>
       <c r="F14" s="2">
-        <v>1.93</v>
+        <v>3.02</v>
       </c>
       <c r="G14" s="2">
-        <v>1.84</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
+        <v>2.44</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
         <v>0</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>22116015</v>
+        <v>22117098</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -1155,80 +1155,80 @@
         <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>2.5</v>
+        <v>2.36</v>
       </c>
       <c r="E15" s="2">
-        <v>2.41</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2">
-        <v>2.4</v>
+        <v>2.06</v>
       </c>
       <c r="G15" s="2">
-        <v>2.25</v>
+        <v>2.13</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
       </c>
       <c r="I15" s="3">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="J15" s="3">
         <v>2</v>
       </c>
       <c r="K15" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="L15" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="M15" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>22116016</v>
+        <v>22117099</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2">
-        <v>2.64</v>
+        <v>3.2</v>
       </c>
       <c r="E16" s="2">
-        <v>2.35</v>
+        <v>2.89</v>
       </c>
       <c r="F16" s="2">
-        <v>2.5299999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="G16" s="2">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2">
-        <v>2</v>
+        <v>2.98</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2.5</v>
       </c>
       <c r="J16" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" s="3">
         <v>2</v>
       </c>
       <c r="L16" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="M16" s="2">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>3.75</v>
+      </c>
+      <c r="M16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>22116017</v>
+        <v>22117100</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -1237,39 +1237,39 @@
         <v>1</v>
       </c>
       <c r="D17" s="2">
-        <v>1.95</v>
+        <v>3.5</v>
       </c>
       <c r="E17" s="2">
-        <v>1.39</v>
+        <v>3.44</v>
       </c>
       <c r="F17" s="2">
-        <v>1.5</v>
+        <v>3.44</v>
       </c>
       <c r="G17" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3.49</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>22116018</v>
+        <v>22117101</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
@@ -1278,39 +1278,39 @@
         <v>1</v>
       </c>
       <c r="D18" s="2">
-        <v>2.4500000000000002</v>
+        <v>2.86</v>
       </c>
       <c r="E18" s="2">
-        <v>2.35</v>
+        <v>3.08</v>
       </c>
       <c r="F18" s="2">
-        <v>2.4</v>
+        <v>3.11</v>
       </c>
       <c r="G18" s="2">
-        <v>2.2999999999999998</v>
+        <v>3.18</v>
       </c>
       <c r="H18" s="3">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="I18" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J18" s="3">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="K18" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>22116020</v>
+        <v>22117102</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
@@ -1319,39 +1319,39 @@
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>1.55</v>
+        <v>3.2</v>
       </c>
       <c r="E19" s="2">
-        <v>1.28</v>
+        <v>3.2</v>
       </c>
       <c r="F19" s="2">
-        <v>1.55</v>
+        <v>3.23</v>
       </c>
       <c r="G19" s="2">
-        <v>1.52</v>
+        <v>3.31</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" s="3">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="J19" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2</v>
+      </c>
+      <c r="L19" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>22116021</v>
+        <v>22117103</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
@@ -1360,39 +1360,39 @@
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>2.31</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
-        <v>2.74</v>
+        <v>2.82</v>
       </c>
       <c r="F20" s="2">
-        <v>2.35</v>
+        <v>2.81</v>
       </c>
       <c r="G20" s="2">
-        <v>1.88</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
-        <v>0</v>
-      </c>
-      <c r="M20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M20" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>22116022</v>
+        <v>22117104</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
@@ -1401,80 +1401,80 @@
         <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>2.67</v>
+        <v>2.14</v>
       </c>
       <c r="E21" s="2">
-        <v>2.2799999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="F21" s="2">
-        <v>2.21</v>
+        <v>1.86</v>
       </c>
       <c r="G21" s="2">
-        <v>2.17</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
         <v>0</v>
       </c>
       <c r="M21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>22116023</v>
+        <v>22117106</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2">
-        <v>2.67</v>
+        <v>3.25</v>
       </c>
       <c r="E22" s="2">
-        <v>2.1</v>
+        <v>3.24</v>
       </c>
       <c r="F22" s="2">
-        <v>2.34</v>
+        <v>3.22</v>
       </c>
       <c r="G22" s="2">
-        <v>2.41</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3.26</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M22" s="3">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22116024</v>
+        <v>22117111</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
@@ -1483,39 +1483,39 @@
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>2.39</v>
+        <v>2.84</v>
       </c>
       <c r="E23" s="2">
-        <v>2.6</v>
+        <v>1.49</v>
       </c>
       <c r="F23" s="2">
-        <v>2.78</v>
+        <v>1.6</v>
       </c>
       <c r="G23" s="2">
-        <v>2.84</v>
-      </c>
-      <c r="H23" s="2">
-        <v>2</v>
-      </c>
-      <c r="I23" s="2">
-        <v>3</v>
-      </c>
-      <c r="J23" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="K23" s="2">
-        <v>2</v>
-      </c>
-      <c r="L23" s="2">
-        <v>3</v>
-      </c>
-      <c r="M23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2.04</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J23" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>22116026</v>
+        <v>22117112</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -1524,66 +1524,66 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>2</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E24" s="2">
-        <v>1.83</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="F24" s="2">
-        <v>1.24</v>
+        <v>1.81</v>
       </c>
       <c r="G24" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>2.02</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>22116027</v>
+        <v>22117114</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
-        <v>3.11</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E25" s="2">
-        <v>3.15</v>
+        <v>1.75</v>
       </c>
       <c r="F25" s="2">
-        <v>3.05</v>
+        <v>1.94</v>
       </c>
       <c r="G25" s="2">
-        <v>2.63</v>
+        <v>2.12</v>
       </c>
       <c r="H25" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I25" s="3">
         <v>2</v>
       </c>
       <c r="J25" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K25" s="3">
         <v>2</v>
@@ -1592,53 +1592,53 @@
         <v>2.5</v>
       </c>
       <c r="M25" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="69" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>22116028</v>
+        <v>22117115</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2">
-        <v>2.67</v>
+        <v>3.02</v>
       </c>
       <c r="E26" s="2">
-        <v>2.96</v>
+        <v>2.66</v>
       </c>
       <c r="F26" s="2">
-        <v>3.03</v>
+        <v>2.68</v>
       </c>
       <c r="G26" s="2">
-        <v>3.06</v>
+        <v>2.68</v>
       </c>
       <c r="H26" s="3">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="I26" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K26" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L26" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M26" s="3">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>22116029</v>
+        <v>22117116</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
@@ -1647,39 +1647,39 @@
         <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>2.5</v>
+        <v>2.77</v>
       </c>
       <c r="E27" s="2">
-        <v>2.65</v>
+        <v>2.82</v>
       </c>
       <c r="F27" s="2">
-        <v>2.76</v>
+        <v>2.97</v>
       </c>
       <c r="G27" s="2">
-        <v>2.84</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2</v>
-      </c>
-      <c r="I27" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="J27" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="K27" s="2">
-        <v>2</v>
-      </c>
-      <c r="L27" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="M27" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>3.12</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J27" s="3">
+        <v>3</v>
+      </c>
+      <c r="K27" s="3">
+        <v>3</v>
+      </c>
+      <c r="L27" s="3">
+        <v>4</v>
+      </c>
+      <c r="M27" s="3">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>22116030</v>
+        <v>22117117</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
@@ -1688,16 +1688,16 @@
         <v>1</v>
       </c>
       <c r="D28" s="2">
-        <v>1.22</v>
+        <v>0.41</v>
       </c>
       <c r="E28" s="2">
-        <v>3.08</v>
+        <v>0.26</v>
       </c>
       <c r="F28" s="2">
-        <v>1.34</v>
+        <v>0.39</v>
       </c>
       <c r="G28" s="2">
-        <v>1.05</v>
+        <v>0.38</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
@@ -1718,9 +1718,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>22116031</v>
+        <v>22117118</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
@@ -1729,39 +1729,39 @@
         <v>1</v>
       </c>
       <c r="D29" s="2">
-        <v>2.78</v>
+        <v>0.9</v>
       </c>
       <c r="E29" s="2">
-        <v>3.08</v>
+        <v>0.79</v>
       </c>
       <c r="F29" s="2">
-        <v>2.97</v>
+        <v>0.61</v>
       </c>
       <c r="G29" s="2">
-        <v>2.89</v>
+        <v>0.8</v>
       </c>
       <c r="H29" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L29" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>22116032</v>
+        <v>22117119</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
@@ -1770,16 +1770,16 @@
         <v>1</v>
       </c>
       <c r="D30" s="2">
-        <v>2.67</v>
+        <v>2.66</v>
       </c>
       <c r="E30" s="2">
-        <v>2.62</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="F30" s="2">
-        <v>2.86</v>
+        <v>2.39</v>
       </c>
       <c r="G30" s="2">
-        <v>2.83</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="H30" s="3">
         <v>2</v>
@@ -1788,21 +1788,21 @@
         <v>2.5</v>
       </c>
       <c r="J30" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K30" s="3">
         <v>2.5</v>
       </c>
       <c r="L30" s="3">
-        <v>2</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="M30" s="3">
+        <v>3.75</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>22116033</v>
+        <v>22117120</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
@@ -1811,39 +1811,39 @@
         <v>1</v>
       </c>
       <c r="D31" s="2">
-        <v>2.25</v>
+        <v>0.36</v>
       </c>
       <c r="E31" s="2">
-        <v>2.76</v>
+        <v>0.24</v>
       </c>
       <c r="F31" s="2">
-        <v>2.78</v>
+        <v>0.59</v>
       </c>
       <c r="G31" s="2">
-        <v>2.65</v>
-      </c>
-      <c r="H31" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="I31" s="3">
-        <v>2</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
-      </c>
-      <c r="K31" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L31" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M31" s="3">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>22116034</v>
+        <v>22117121</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
@@ -1852,80 +1852,80 @@
         <v>1</v>
       </c>
       <c r="D32" s="2">
-        <v>2.65</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E32" s="2">
-        <v>2.8</v>
+        <v>2.04</v>
       </c>
       <c r="F32" s="2">
-        <v>2.87</v>
+        <v>1.99</v>
       </c>
       <c r="G32" s="2">
-        <v>2.87</v>
+        <v>2.23</v>
       </c>
       <c r="H32" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I32" s="3">
         <v>2.5</v>
       </c>
       <c r="J32" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="K32" s="3">
         <v>2.5</v>
       </c>
       <c r="L32" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M32" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>22116035</v>
+        <v>22117122</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2">
-        <v>1.95</v>
+        <v>2.39</v>
       </c>
       <c r="E33" s="2">
-        <v>1.56</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="F33" s="2">
-        <v>1.64</v>
+        <v>2.56</v>
       </c>
       <c r="G33" s="2">
-        <v>1.64</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
-        <v>0</v>
-      </c>
-      <c r="J33" s="2">
-        <v>0</v>
+        <v>2.69</v>
+      </c>
+      <c r="H33" s="3">
+        <v>2</v>
+      </c>
+      <c r="I33" s="3">
+        <v>2</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2</v>
       </c>
       <c r="K33" s="3">
         <v>2</v>
       </c>
-      <c r="L33" s="2">
-        <v>0</v>
-      </c>
-      <c r="M33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="L33" s="3">
+        <v>3</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>22116038</v>
+        <v>22117124</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>33</v>
@@ -1934,16 +1934,16 @@
         <v>1</v>
       </c>
       <c r="D34" s="2">
-        <v>2.06</v>
+        <v>2.64</v>
       </c>
       <c r="E34" s="2">
-        <v>2.4900000000000002</v>
+        <v>2.02</v>
       </c>
       <c r="F34" s="2">
-        <v>2.57</v>
+        <v>2.14</v>
       </c>
       <c r="G34" s="2">
-        <v>2.5299999999999998</v>
+        <v>2.02</v>
       </c>
       <c r="H34" s="3">
         <v>2</v>
@@ -1958,97 +1958,97 @@
         <v>2</v>
       </c>
       <c r="L34" s="3">
-        <v>3</v>
-      </c>
-      <c r="M34" s="2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="M34" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>22116039</v>
+        <v>22117125</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2">
-        <v>3.05</v>
+        <v>2.83</v>
       </c>
       <c r="E35" s="2">
-        <v>3.06</v>
+        <v>2.37</v>
       </c>
       <c r="F35" s="2">
-        <v>2.87</v>
+        <v>2.39</v>
       </c>
       <c r="G35" s="2">
-        <v>2.72</v>
+        <v>2.62</v>
       </c>
       <c r="H35" s="3">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I35" s="3">
         <v>2.5</v>
       </c>
       <c r="J35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K35" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L35" s="3">
         <v>3</v>
       </c>
-      <c r="M35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="M35" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>22116040</v>
+        <v>22117126</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="2">
-        <v>2.94</v>
+        <v>2.95</v>
       </c>
       <c r="E36" s="2">
-        <v>2.91</v>
+        <v>2.87</v>
       </c>
       <c r="F36" s="2">
-        <v>3.11</v>
+        <v>2.85</v>
       </c>
       <c r="G36" s="2">
-        <v>3.03</v>
+        <v>2.87</v>
       </c>
       <c r="H36" s="3">
         <v>2.5</v>
       </c>
       <c r="I36" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J36" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K36" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="L36" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="M36" s="3">
-        <v>3</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>22116047</v>
+        <v>22118002</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>36</v>
@@ -2057,80 +2057,80 @@
         <v>1</v>
       </c>
       <c r="D37" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.68</v>
       </c>
       <c r="E37" s="2">
-        <v>2.12</v>
+        <v>1.88</v>
       </c>
       <c r="F37" s="2">
-        <v>2.2599999999999998</v>
+        <v>1.88</v>
       </c>
       <c r="G37" s="2">
-        <v>2.31</v>
-      </c>
-      <c r="H37" s="2">
-        <v>2.5</v>
+        <v>1.44</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K37" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="L37" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M37" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>22116049</v>
+        <v>22118004</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="2">
-        <v>2.63</v>
+        <v>3.05</v>
       </c>
       <c r="E38" s="2">
-        <v>3.08</v>
+        <v>3</v>
       </c>
       <c r="F38" s="2">
-        <v>3.09</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G38" s="2">
-        <v>3.01</v>
+        <v>2.4</v>
       </c>
       <c r="H38" s="3">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I38" s="3">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="J38" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K38" s="3">
         <v>3</v>
       </c>
       <c r="L38" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M38" s="3">
         <v>3.75</v>
       </c>
-      <c r="M38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>22116051</v>
+        <v>22118005</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>38</v>
@@ -2139,39 +2139,39 @@
         <v>1</v>
       </c>
       <c r="D39" s="2">
-        <v>2.69</v>
+        <v>2.84</v>
       </c>
       <c r="E39" s="2">
-        <v>2.91</v>
+        <v>2.79</v>
       </c>
       <c r="F39" s="2">
-        <v>3.01</v>
+        <v>2.06</v>
       </c>
       <c r="G39" s="2">
-        <v>2.96</v>
+        <v>2.4</v>
       </c>
       <c r="H39" s="3">
-        <v>3</v>
-      </c>
-      <c r="I39" s="3">
-        <v>3</v>
-      </c>
-      <c r="J39" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="K39" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L39" s="3">
-        <v>3.75</v>
-      </c>
-      <c r="M39" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>22116052</v>
+        <v>22118006</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
@@ -2180,28 +2180,28 @@
         <v>1</v>
       </c>
       <c r="D40" s="2">
-        <v>3.11</v>
+        <v>3.07</v>
       </c>
       <c r="E40" s="2">
-        <v>3.24</v>
+        <v>3.01</v>
       </c>
       <c r="F40" s="2">
-        <v>3.28</v>
+        <v>3.09</v>
       </c>
       <c r="G40" s="2">
-        <v>3.22</v>
+        <v>3.07</v>
       </c>
       <c r="H40" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="I40" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J40" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K40" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L40" s="3">
         <v>3</v>
@@ -2210,9 +2210,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>22116053</v>
+        <v>22118007</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
@@ -2221,39 +2221,39 @@
         <v>1</v>
       </c>
       <c r="D41" s="2">
-        <v>2.36</v>
+        <v>3.25</v>
       </c>
       <c r="E41" s="2">
-        <v>2.7</v>
+        <v>3.33</v>
       </c>
       <c r="F41" s="2">
-        <v>2.64</v>
+        <v>3.45</v>
       </c>
       <c r="G41" s="2">
-        <v>2.66</v>
-      </c>
-      <c r="H41" s="2">
-        <v>2</v>
-      </c>
-      <c r="I41" s="2">
-        <v>2</v>
-      </c>
-      <c r="J41" s="2">
-        <v>2</v>
-      </c>
-      <c r="K41" s="2">
-        <v>2</v>
-      </c>
-      <c r="L41" s="2">
-        <v>3</v>
-      </c>
-      <c r="M41" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3.43</v>
+      </c>
+      <c r="H41" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="I41" s="3">
+        <v>4</v>
+      </c>
+      <c r="J41" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="K41" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="L41" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M41" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>22116056</v>
+        <v>22118008</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
@@ -2262,80 +2262,80 @@
         <v>1</v>
       </c>
       <c r="D42" s="2">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="E42" s="2">
-        <v>2.46</v>
+        <v>1.69</v>
       </c>
       <c r="F42" s="2">
-        <v>2.72</v>
+        <v>1.75</v>
       </c>
       <c r="G42" s="2">
-        <v>2.68</v>
-      </c>
-      <c r="H42" s="2">
-        <v>2</v>
+        <v>1.9</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="K42" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L42" s="2">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="69" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>22116057</v>
+        <v>22118009</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2">
-        <v>2.56</v>
+        <v>3.39</v>
       </c>
       <c r="E43" s="2">
-        <v>2.29</v>
+        <v>3.44</v>
       </c>
       <c r="F43" s="2">
-        <v>2.2000000000000002</v>
+        <v>3.46</v>
       </c>
       <c r="G43" s="2">
-        <v>2.14</v>
+        <v>3.3</v>
       </c>
       <c r="H43" s="3">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="I43" s="3">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="J43" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K43" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L43" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="M43" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>22116071</v>
+        <v>22118010</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>43</v>
@@ -2344,39 +2344,39 @@
         <v>1</v>
       </c>
       <c r="D44" s="2">
-        <v>2.06</v>
+        <v>2.89</v>
       </c>
       <c r="E44" s="2">
-        <v>2.44</v>
+        <v>2.79</v>
       </c>
       <c r="F44" s="2">
-        <v>2.5099999999999998</v>
+        <v>2.94</v>
       </c>
       <c r="G44" s="2">
-        <v>2.39</v>
+        <v>2.73</v>
       </c>
       <c r="H44" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="I44" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="J44" s="3">
         <v>3</v>
       </c>
       <c r="K44" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="L44" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M44" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>22116075</v>
+        <v>22118011</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
@@ -2385,25 +2385,25 @@
         <v>1</v>
       </c>
       <c r="D45" s="2">
-        <v>2.17</v>
+        <v>2.82</v>
       </c>
       <c r="E45" s="2">
-        <v>2.38</v>
+        <v>2.85</v>
       </c>
       <c r="F45" s="2">
-        <v>2.46</v>
+        <v>2.87</v>
       </c>
       <c r="G45" s="2">
-        <v>2.4900000000000002</v>
+        <v>2.81</v>
       </c>
       <c r="H45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K45" s="3">
         <v>3</v>
@@ -2412,12 +2412,12 @@
         <v>2.5</v>
       </c>
       <c r="M45" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>22116078</v>
+        <v>22118012</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
@@ -2426,39 +2426,39 @@
         <v>1</v>
       </c>
       <c r="D46" s="2">
-        <v>2.5</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E46" s="2">
-        <v>2.7</v>
+        <v>2.33</v>
       </c>
       <c r="F46" s="2">
-        <v>2.84</v>
+        <v>1.7</v>
       </c>
       <c r="G46" s="2">
-        <v>2.84</v>
+        <v>1.9</v>
       </c>
       <c r="H46" s="3">
         <v>2</v>
       </c>
       <c r="I46" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="J46" s="3">
-        <v>2</v>
-      </c>
-      <c r="K46" s="3">
-        <v>2</v>
-      </c>
-      <c r="L46" s="3">
-        <v>2</v>
-      </c>
-      <c r="M46" s="3">
-        <v>2.5</v>
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>22116079</v>
+        <v>22118021</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>46</v>
@@ -2467,121 +2467,121 @@
         <v>1</v>
       </c>
       <c r="D47" s="2">
-        <v>2.4</v>
+        <v>2.98</v>
       </c>
       <c r="E47" s="2">
-        <v>2.31</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="F47" s="2">
-        <v>1.84</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="G47" s="2">
-        <v>1.59</v>
+        <v>2.38</v>
       </c>
       <c r="H47" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J47" s="3">
-        <v>0</v>
-      </c>
-      <c r="K47" s="2">
-        <v>0</v>
-      </c>
-      <c r="L47" s="2">
-        <v>0</v>
+        <v>2.5</v>
+      </c>
+      <c r="K47" s="3">
+        <v>3</v>
+      </c>
+      <c r="L47" s="3">
+        <v>2</v>
       </c>
       <c r="M47" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>22116086</v>
+        <v>22118022</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="2">
-        <v>2.08</v>
+        <v>3.16</v>
       </c>
       <c r="E48" s="2">
-        <v>2.5299999999999998</v>
+        <v>3.32</v>
       </c>
       <c r="F48" s="2">
-        <v>2.64</v>
+        <v>3.29</v>
       </c>
       <c r="G48" s="2">
-        <v>2.65</v>
-      </c>
-      <c r="H48" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="I48" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="J48" s="2">
-        <v>3</v>
-      </c>
-      <c r="K48" s="2">
-        <v>2</v>
-      </c>
-      <c r="L48" s="2">
-        <v>2</v>
-      </c>
-      <c r="M48" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+        <v>3.23</v>
+      </c>
+      <c r="H48" s="3">
+        <v>3</v>
+      </c>
+      <c r="I48" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J48" s="3">
+        <v>3</v>
+      </c>
+      <c r="K48" s="3">
+        <v>2</v>
+      </c>
+      <c r="L48" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M48" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>22116087</v>
+        <v>22118024</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2">
-        <v>2.97</v>
+        <v>3.18</v>
       </c>
       <c r="E49" s="2">
-        <v>2.96</v>
+        <v>2.88</v>
       </c>
       <c r="F49" s="2">
-        <v>2.95</v>
+        <v>2.74</v>
       </c>
       <c r="G49" s="2">
-        <v>2.95</v>
+        <v>2.79</v>
       </c>
       <c r="H49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L49" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M49" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>22116088</v>
+        <v>22118025</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>49</v>
@@ -2590,34 +2590,34 @@
         <v>1</v>
       </c>
       <c r="D50" s="2">
-        <v>2</v>
+        <v>3.16</v>
       </c>
       <c r="E50" s="2">
-        <v>2.75</v>
+        <v>2.77</v>
       </c>
       <c r="F50" s="2">
-        <v>2.39</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2">
-        <v>2.36</v>
+        <v>2.72</v>
       </c>
       <c r="H50" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="I50" s="3">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J50" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K50" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L50" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="M50" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>